<commit_message>
cypress 10 cucumber v11
</commit_message>
<xml_diff>
--- a/cypress/fixtures/xlsx/login.xlsx
+++ b/cypress/fixtures/xlsx/login.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wassim\Desktop\Cypress\Cypress10-Cucumber-Typescript-Xpath\cypress\fixtures\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE88C17-0A2D-47E8-9D15-F2343C83A059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DCE036-A003-46AB-999A-0CE36360E9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -486,63 +486,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="B1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3">
+      <c r="C2" s="3">
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5">
+      <c r="C3" s="5">
         <v>456</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
+      <c r="C4" s="5">
         <v>789</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="7">
+      <c r="C5" s="7">
         <v>753</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{6C5F6021-DC54-459C-A158-EF4057A2A7EE}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{24A649A5-9A88-40CB-B9B3-B3032E1FF35D}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{3300B896-1A40-43EF-B380-8CAEBEB13980}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{77B9CF3F-4327-4FF5-9D87-D9A4DF5173CD}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{6C5F6021-DC54-459C-A158-EF4057A2A7EE}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{24A649A5-9A88-40CB-B9B3-B3032E1FF35D}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{3300B896-1A40-43EF-B380-8CAEBEB13980}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{77B9CF3F-4327-4FF5-9D87-D9A4DF5173CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>

</xml_diff>

<commit_message>
cypress 10 cucumber v12
</commit_message>
<xml_diff>
--- a/cypress/fixtures/xlsx/login.xlsx
+++ b/cypress/fixtures/xlsx/login.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wassim\Desktop\Cypress\Cypress10-Cucumber-Typescript-Xpath\cypress\fixtures\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DCE036-A003-46AB-999A-0CE36360E9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391DB1EF-0C99-4B19-8CA3-E53BF03AAA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="invalid-users" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -49,16 +49,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -73,16 +65,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -109,7 +130,48 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -119,7 +181,33 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -127,66 +215,6 @@
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -194,17 +222,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -488,52 +517,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="3">
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>456</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>789</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="6" t="s">
+    <row r="5" spans="2:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>753</v>
       </c>
     </row>

</xml_diff>